<commit_message>
Update Vis Tool + Teams Data
</commit_message>
<xml_diff>
--- a/data/CurrentSeason/DAL.xlsx
+++ b/data/CurrentSeason/DAL.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,6 +2912,67 @@
       </c>
       <c r="S40" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>45304</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D41" t="n">
+        <v>108</v>
+      </c>
+      <c r="E41" t="n">
+        <v>89.7</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="G41" t="n">
+        <v>11.7</v>
+      </c>
+      <c r="H41" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="J41" t="n">
+        <v>120.5</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>NOP</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>118</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="N41" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="O41" t="n">
+        <v>35.9</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.354</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>131.6</v>
+      </c>
+      <c r="R41" t="n">
+        <v>1</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2925,7 +2986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2952,7 +3013,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45304</v>
+        <v>45306</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2965,24 +3026,24 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45306</v>
+        <v>45308</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45308</v>
+        <v>45310</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -2991,24 +3052,24 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45310</v>
+        <v>45313</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45313</v>
+        <v>45315</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>PHO</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -3017,37 +3078,37 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45315</v>
+        <v>45317</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PHO</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45317</v>
+        <v>45318</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45318</v>
+        <v>45320</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -3056,50 +3117,50 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45320</v>
+        <v>45322</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45322</v>
+        <v>45325</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45325</v>
+        <v>45327</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45327</v>
+        <v>45328</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>BRK</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -3108,11 +3169,11 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BRK</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -3121,24 +3182,24 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45332</v>
+        <v>45334</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -3147,11 +3208,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45334</v>
+        <v>45336</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -3160,11 +3221,11 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45336</v>
+        <v>45344</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>PHO</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -3173,24 +3234,24 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45344</v>
+        <v>45347</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PHO</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45347</v>
+        <v>45349</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -3199,11 +3260,11 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -3212,11 +3273,11 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45350</v>
+        <v>45352</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -3225,24 +3286,24 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45352</v>
+        <v>45354</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45354</v>
+        <v>45356</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -3251,11 +3312,11 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45356</v>
+        <v>45358</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -3264,24 +3325,24 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45358</v>
+        <v>45360</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45360</v>
+        <v>45362</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -3290,72 +3351,72 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45362</v>
+        <v>45364</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45365</v>
+        <v>45368</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45368</v>
+        <v>45370</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45370</v>
+        <v>45372</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45372</v>
+        <v>45376</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3363,16 +3424,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -3381,7 +3442,7 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45377</v>
+        <v>45380</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3394,11 +3455,11 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45380</v>
+        <v>45382</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -3407,24 +3468,24 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45382</v>
+        <v>45384</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45384</v>
+        <v>45387</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -3433,11 +3494,11 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45387</v>
+        <v>45389</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -3446,24 +3507,24 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45389</v>
+        <v>45391</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>CHO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45391</v>
+        <v>45392</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CHO</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -3472,40 +3533,27 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45392</v>
+        <v>45394</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45394</v>
+        <v>45396</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
-        <v>45396</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>OKC</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>